<commit_message>
Saca ambas distancias y las suma
</commit_message>
<xml_diff>
--- a/reviews_sentiment.xlsx
+++ b/reviews_sentiment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vdgp_\OneDrive\Escritorio\QCEI\septimo\Minerias de datos\kNearestNeighbor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A96E9F-246D-4A69-86A7-A8D1771C3810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C2C42E-C7FE-4812-8C15-6EAA3058F7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -503,7 +503,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,7 +548,7 @@
         <v>9</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <v>-0.48638925497678998</v>
@@ -571,7 +571,7 @@
         <v>9</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G3">
         <v>-0.58618747273392002</v>
@@ -594,7 +594,7 @@
         <v>9</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G4">
         <v>-0.60224027478572995</v>
@@ -617,7 +617,7 @@
         <v>9</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G5">
         <v>-0.61627120566332005</v>
@@ -640,7 +640,7 @@
         <v>9</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6">
         <v>-0.65178360084621001</v>
@@ -663,7 +663,7 @@
         <v>9</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <v>-0.72044292561513001</v>
@@ -686,7 +686,7 @@
         <v>9</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G8">
         <v>-0.72682540878887003</v>
@@ -709,7 +709,7 @@
         <v>9</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G9">
         <v>-0.73676947090928002</v>
@@ -732,7 +732,7 @@
         <v>9</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10">
         <v>-0.76528370259873002</v>
@@ -755,7 +755,7 @@
         <v>9</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11">
         <v>-0.79796123004129005</v>
@@ -778,7 +778,7 @@
         <v>9</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G12">
         <v>-0.83348759799377004</v>
@@ -801,7 +801,7 @@
         <v>9</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G13">
         <v>-0.83846653151519002</v>
@@ -824,7 +824,7 @@
         <v>9</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G14">
         <v>-0.88855903504626998</v>
@@ -847,7 +847,7 @@
         <v>9</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G15">
         <v>-1.0026961447431</v>
@@ -870,7 +870,7 @@
         <v>9</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G16">
         <v>-1.0832692852162999</v>
@@ -893,7 +893,7 @@
         <v>9</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G17">
         <v>-1.0981097654005001</v>
@@ -916,7 +916,7 @@
         <v>9</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G18">
         <v>-1.1044687905632</v>
@@ -939,7 +939,7 @@
         <v>9</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G19">
         <v>-1.1122230773374999</v>
@@ -962,7 +962,7 @@
         <v>9</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G20">
         <v>-1.2754114957138001</v>

</xml_diff>